<commit_message>
Updating new Warrant IEPDs
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Warrant_Issued_Reporting/artifacts/service_model/information_model/IEPD/documentation/Mapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Warrant_Issued_Reporting/artifacts/service_model/information_model/IEPD/documentation/Mapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-27700" yWindow="6520" windowWidth="25600" windowHeight="15040" tabRatio="500"/>
+    <workbookView xWindow="-26960" yWindow="6880" windowWidth="25600" windowHeight="15040" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Warrant Issued Report" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="236">
   <si>
     <t>CLASS</t>
   </si>
@@ -125,12 +125,6 @@
     <t>Address Category Text</t>
   </si>
   <si>
-    <t>Address County Name</t>
-  </si>
-  <si>
-    <t>Address County Code</t>
-  </si>
-  <si>
     <t>Street Number Text</t>
   </si>
   <si>
@@ -170,9 +164,6 @@
     <t>Law Enforcement ORI</t>
   </si>
   <si>
-    <t>Complaint Number</t>
-  </si>
-  <si>
     <t>Offense Code Text</t>
   </si>
   <si>
@@ -197,12 +188,6 @@
     <t>Person Record Number</t>
   </si>
   <si>
-    <t>Vehicle Record Number</t>
-  </si>
-  <si>
-    <t>A system record number for a person.</t>
-  </si>
-  <si>
     <t>A code representing the extent to which a warrant will be broadcast.</t>
   </si>
   <si>
@@ -215,21 +200,12 @@
     <t>ORI of the warrant issuing agency</t>
   </si>
   <si>
-    <t>Charge Agency Record ID??</t>
-  </si>
-  <si>
     <t>Caution Code Text</t>
   </si>
   <si>
     <t>ID of the person who entered the warrant</t>
   </si>
   <si>
-    <t>The system record number of a person</t>
-  </si>
-  <si>
-    <t>Vehicle Record Expiration Date</t>
-  </si>
-  <si>
     <t>Warrant Appearance Bail Amount</t>
   </si>
   <si>
@@ -248,12 +224,6 @@
     <t>A miscellaneous unique identification assigned to a person record.</t>
   </si>
   <si>
-    <t>A unique identification assigned to a vehicle record.</t>
-  </si>
-  <si>
-    <t>The expiration date of a vehicle record.</t>
-  </si>
-  <si>
     <t>Additional information about a vehicle.</t>
   </si>
   <si>
@@ -266,9 +236,6 @@
     <t>True if a subjectcan be extradited; false otherwise.</t>
   </si>
   <si>
-    <t>Prosecution Warrant Code Text</t>
-  </si>
-  <si>
     <t>A code representing a kind of limitation placed on the extradition of a subject from an area outside the immediate jurisdiction of the issuing court</t>
   </si>
   <si>
@@ -413,9 +380,6 @@
     <t>Excessive Rust</t>
   </si>
   <si>
-    <t>V345678</t>
-  </si>
-  <si>
     <t>LP4365-0234</t>
   </si>
   <si>
@@ -437,9 +401,6 @@
     <t>Michigan</t>
   </si>
   <si>
-    <t>Taylor</t>
-  </si>
-  <si>
     <t>PN3929593</t>
   </si>
   <si>
@@ -461,9 +422,6 @@
     <t>SAME AS ELEMENT IN PERSON CLASS</t>
   </si>
   <si>
-    <t>Citizenship Code Text</t>
-  </si>
-  <si>
     <t>Vehicle Primary Color Code Text</t>
   </si>
   <si>
@@ -479,18 +437,9 @@
     <t>Vehicle Style Code Text</t>
   </si>
   <si>
-    <t>Race Code Text</t>
-  </si>
-  <si>
-    <t>Ethnicity Code Text</t>
-  </si>
-  <si>
     <t>Eye Color Code Text</t>
   </si>
   <si>
-    <t>Sex Code Text</t>
-  </si>
-  <si>
     <t>Skin Tone Code Text</t>
   </si>
   <si>
@@ -503,36 +452,15 @@
     <t>Physical Feature Category Code Text</t>
   </si>
   <si>
-    <t>wir-doc:WarrantIssuedReport/nc:Vehicle[@structures:id=/wir-doc:WarrantIssuedReport/nc:PersonConveyanceAssociation/nc:Conveyance/@structures:ref]/nc:ConveyanceColorPrimaryText</t>
-  </si>
-  <si>
-    <t>wir-doc:WarrantIssuedReport/nc:Vehicle[@structures:id=/wir-doc:WarrantIssuedReport/nc:PersonConveyanceAssociation/nc:Conveyance/@structures:ref]/nc:ConveyanceColorSecondaryText</t>
-  </si>
-  <si>
-    <t>wir-doc:WarrantIssuedReport/nc:Vehicle[@structures:id=/wir-doc:WarrantIssuedReport/nc:PersonConveyanceAssociation/nc:Conveyance/@structures:ref]/nc:ItemMakeName</t>
-  </si>
-  <si>
-    <t>wir-doc:WarrantIssuedReport/nc:Vehicle[@structures:id=/wir-doc:WarrantIssuedReport/nc:PersonConveyanceAssociation/nc:Conveyance/@structures:ref]/nc:ItemModelName</t>
-  </si>
-  <si>
     <t>wir-doc:WarrantIssuedReport/nc:Vehicle[@structures:id=/wir-doc:WarrantIssuedReport/nc:PersonConveyanceAssociation/nc:Conveyance/@structures:ref]/nc:ItemModelYearDate</t>
   </si>
   <si>
-    <t>wir-doc:WarrantIssuedReport/nc:Vehicle[@structures:id=/wir-doc:WarrantIssuedReport/nc:PersonConveyanceAssociation/nc:Conveyance/@structures:ref]/nc:ItemStyleText</t>
-  </si>
-  <si>
     <t>wir-doc:WarrantIssuedReport/nc:Vehicle[@structures:id=/wir-doc:WarrantIssuedReport/nc:PersonConveyanceAssociation/nc:Conveyance/@structures:ref]/nc:VehicleIdentification/nc:IdentificationID</t>
   </si>
   <si>
-    <t>wir-doc:WarrantIssuedReport/nc:Vehicle[@structures:id=/wir-doc:WarrantIssuedReport/nc:PersonConveyanceAssociation/nc:Conveyance/@structures:ref]/wir-ext:VehicleRecordExpirationDate/nc:Date</t>
-  </si>
-  <si>
     <t>wir-doc:WarrantIssuedReport/nc:Vehicle[@structures:id=/wir-doc:WarrantIssuedReport/nc:PersonConveyanceAssociation/nc:Conveyance/@structures:ref]/wir-ext:VehicleAdditionalInformationText</t>
   </si>
   <si>
-    <t>wir-doc:WarrantIssuedReport/nc:Vehicle[@structures:id=/wir-doc:WarrantIssuedReport/nc:PersonConveyanceAssociation/nc:Conveyance/@structures:ref]/wir-ext:VehicleRecordIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
     <t>wir-doc:WarrantIssuedReport/nc:Person/nc:PersonName/nc:PersonGivenName</t>
   </si>
   <si>
@@ -548,24 +476,12 @@
     <t>wir-doc:WarrantIssuedReport/nc:Person/nc:PersonName/nc:PersonFullName</t>
   </si>
   <si>
-    <t>wir-doc:WarrantIssuedReport/nc:Person/nc:PersonCitizenshipText</t>
-  </si>
-  <si>
     <t>wir-doc:WarrantIssuedReport/nc:Person/nc:PersonBirthDate/nc:Date</t>
   </si>
   <si>
-    <t>wir-doc:WarrantIssuedReport/nc:Person/nc:PersonEthnicityText</t>
-  </si>
-  <si>
-    <t>wir-doc:WarrantIssuedReport/nc:Person/nc:PersonRaceText</t>
-  </si>
-  <si>
     <t>wir-doc:WarrantIssuedReport/nc:Person/nc:PersonEyeColorText</t>
   </si>
   <si>
-    <t>wir-doc:WarrantIssuedReport/nc:Person/nc:PersonSexText</t>
-  </si>
-  <si>
     <t>wir-doc:WarrantIssuedReport/nc:Person/j:PersonAugmentation/j:PersonFBIIdentification/nc:IdentificationID</t>
   </si>
   <si>
@@ -599,9 +515,6 @@
     <t>wir-doc:WarrantIssuedReport/nc:Person/wir-ext:PersonMiscellaneousRecordIdentification/nc:IdentificationID</t>
   </si>
   <si>
-    <t>wir-doc:WarrantIssuedReport/nc:Person/wir-ext:PersonRecordIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
     <t>wir-doc:WarrantIssuedReport/nc:Person/wir-ext:PersonAdditionalInformationText</t>
   </si>
   <si>
@@ -665,12 +578,6 @@
     <t>wir-doc:WarrantIssuedReport/nc:ContactInformation/nc:ContactMailingAddress[@structures:id=/wir-doc:WarrantIssuedReport/nc:ContactInformationAssociation/nc:ContactInformation/nc:ContactMailingAddress/@structures:ref]/nc:LocationStateName</t>
   </si>
   <si>
-    <t>wir-doc:WarrantIssuedReport/nc:ContactInformation/nc:ContactMailingAddress[@structures:id=/wir-doc:WarrantIssuedReport/nc:ContactInformationAssociation/nc:ContactInformation/nc:ContactMailingAddress/@structures:ref]/nc:LocationCountyName</t>
-  </si>
-  <si>
-    <t>wir-doc:WarrantIssuedReport/nc:ContactInformation/nc:ContactMailingAddress[@structures:id=/wir-doc:WarrantIssuedReport/nc:ContactInformationAssociation/nc:ContactInformation/nc:ContactMailingAddress/@structures:ref]/nc:LocationCountyCode</t>
-  </si>
-  <si>
     <t>wir-doc:WarrantIssuedReport/nc:ContactInformation/nc:ContactMailingAddress[@structures:id=/wir-doc:WarrantIssuedReport/nc:ContactInformationAssociation/nc:ContactInformation/nc:ContactMailingAddress/@structures:ref]/nc:LocationPostalCode</t>
   </si>
   <si>
@@ -701,9 +608,6 @@
     <t>wir-doc:WarrantIssuedReport/j:Warrant[@structures:id=/wir-doc:WarrantIssuedReport/j:ActivityWarrantAssociation/j:Warrant/@structures:ref]/j:CourtOrderRequestEntity/nc:EntityPerson/wir-ext:PersonEmployeeIdentification/nc:IdentificationID</t>
   </si>
   <si>
-    <t>wir-doc:WarrantIssuedReport/j:Warrant[@structures:id=/wir-doc:WarrantIssuedReport/j:ActivityWarrantAssociation/j:Warrant/@structures:ref]/wir-ext:WarrantAugmentation/wir-ext:ProsecutionWarrantCodeText</t>
-  </si>
-  <si>
     <t>wir-doc:WarrantIssuedReport/j:Warrant[@structures:id=/wir-doc:WarrantIssuedReport/j:ActivityWarrantAssociation/j:Warrant/@structures:ref]/wir-ext:WarrantAugmentation/wir-ext:PersonRecordIdentification/nc:IdentificationID</t>
   </si>
   <si>
@@ -716,42 +620,12 @@
     <t>war-doc:WarrantAcceptedReport/nc:Person[@structures:id=/war-doc:WarrantAcceptedReport/j:Warrant/j:CourtOrderDesignatedSubject/nc:RoleOfPerson/@structures:ref]/nc:PersonName/nc:PersonGivenName</t>
   </si>
   <si>
-    <t>war-doc:WarrantAcceptedReport/nc:Person[@structures:id=/war-doc:WarrantAcceptedReport/j:Warrant/j:CourtOrderDesignatedSubject/nc:RoleOfPerson/@structures:ref]/nc:PersonName/nc:PersonMiddleName</t>
-  </si>
-  <si>
-    <t>war-doc:WarrantAcceptedReport/nc:Person[@structures:id=/war-doc:WarrantAcceptedReport/j:Warrant/j:CourtOrderDesignatedSubject/nc:RoleOfPerson/@structures:ref]/nc:PersonName/nc:PersonSurName</t>
-  </si>
-  <si>
-    <t>war-doc:WarrantAcceptedReport/nc:Person[@structures:id=/war-doc:WarrantAcceptedReport/j:Warrant/j:CourtOrderDesignatedSubject/nc:RoleOfPerson/@structures:ref]/nc:PersonName/nc:PersonNameSuffixText</t>
-  </si>
-  <si>
-    <t>war-doc:WarrantAcceptedReport/nc:Person[@structures:id=/war-doc:WarrantAcceptedReport/j:Warrant/j:CourtOrderDesignatedSubject/nc:RoleOfPerson/@structures:ref]/nc:PersonBirthDate/nc:Date</t>
-  </si>
-  <si>
-    <t>war-doc:WarrantAcceptedReport/nc:Person[@structures:id=/war-doc:WarrantAcceptedReport/j:Warrant/j:CourtOrderDesignatedSubject/nc:RoleOfPerson/@structures:ref]/nc:PersonRaceText</t>
-  </si>
-  <si>
-    <t>war-doc:WarrantAcceptedReport/nc:Person[@structures:id=/war-doc:WarrantAcceptedReport/j:Warrant/j:CourtOrderDesignatedSubject/nc:RoleOfPerson/@structures:ref]/nc:PersonSexText</t>
-  </si>
-  <si>
-    <t>war-doc:WarrantAcceptedReport/nc:Person[@structures:id=/war-doc:WarrantAcceptedReport/j:Warrant/j:CourtOrderDesignatedSubject/nc:RoleOfPerson/@structures:ref]/wir-ext:PersonRecordIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
-    <t>war-doc:WarrantAcceptedReport/j:Warrant/j:CourtOrderEnforcementAgency/j:OrganizationAugmentation/j:OrganizationORIIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
-    <t>war-doc:WarrantAcceptedReport/j:Warrant/j:CourtOrderRequestEntity/nc:EntityPerson/wir-ext:PersonEmployeeIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
     <t>Criminal Tracking Number</t>
   </si>
   <si>
     <t>ISO</t>
   </si>
   <si>
-    <t>w, h n</t>
-  </si>
-  <si>
     <t xml:space="preserve">State ID </t>
   </si>
   <si>
@@ -764,13 +638,97 @@
     <t>NCIC</t>
   </si>
   <si>
-    <t>LEAgencyRecordIdentification</t>
-  </si>
-  <si>
-    <t>Modified Warrant</t>
-  </si>
-  <si>
-    <t>REMOVE</t>
+    <t>AgencyRecordIdentification</t>
+  </si>
+  <si>
+    <t>wir-doc:WarrantIssuedReport/nc:Person/nc:PersonCitizenshipISO3166Alpha2Code</t>
+  </si>
+  <si>
+    <t>wir-doc:WarrantIssuedReport/nc:Person/nc:PersonEthnicityCode</t>
+  </si>
+  <si>
+    <t>Citizenship Code</t>
+  </si>
+  <si>
+    <t>Ethnicity Code</t>
+  </si>
+  <si>
+    <t>Race Code</t>
+  </si>
+  <si>
+    <t>wir-doc:WarrantIssuedReport/nc:Person/nc:PersonRaceCode</t>
+  </si>
+  <si>
+    <t>Sex Code</t>
+  </si>
+  <si>
+    <t>wir-doc:WarrantIssuedReport/nc:Person/nc:PersonSexCode</t>
+  </si>
+  <si>
+    <t>SID56567</t>
+  </si>
+  <si>
+    <t>wir-doc:WarrantIssuedReport/nc:Person/nc:PersonStateIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>wir-doc:WarrantIssuedReport/nc:Vehicle[@structures:id=/wir-doc:WarrantIssuedReport/nc:PersonConveyanceAssociation/nc:Conveyance/@structures:ref]/nc:ConveyanceColorPrimaryCode</t>
+  </si>
+  <si>
+    <t>wir-doc:WarrantIssuedReport/nc:Vehicle[@structures:id=/wir-doc:WarrantIssuedReport/nc:PersonConveyanceAssociation/nc:Conveyance/@structures:ref]/nc:ConveyanceColorSecondaryCode</t>
+  </si>
+  <si>
+    <t>wir-doc:WarrantIssuedReport/nc:Vehicle[@structures:id=/wir-doc:WarrantIssuedReport/nc:PersonConveyanceAssociation/nc:Conveyance/@structures:ref]/j:VehicleMakeCode</t>
+  </si>
+  <si>
+    <t>DIA</t>
+  </si>
+  <si>
+    <t>wir-doc:WarrantIssuedReport/nc:Vehicle[@structures:id=/wir-doc:WarrantIssuedReport/nc:PersonConveyanceAssociation/nc:Conveyance/@structures:ref]/j:VehicleModelCode</t>
+  </si>
+  <si>
+    <t>wir-doc:WarrantIssuedReport/nc:Vehicle[@structures:id=/wir-doc:WarrantIssuedReport/nc:PersonConveyanceAssociation/nc:Conveyance/@structures:ref]/j:VehicleStyleCode</t>
+  </si>
+  <si>
+    <t>wir-doc:WarrantIssuedReport/j:Warrant[@structures:id=/wir-doc:WarrantIssuedReport/j:ActivityWarrantAssociation/j:Warrant/@structures:ref]/wir-ext:WarrantAugmentation/wir-ext:CriminalTrackingNumber</t>
+  </si>
+  <si>
+    <t>OCA</t>
+  </si>
+  <si>
+    <t>OCA4576</t>
+  </si>
+  <si>
+    <t>wir-doc:WarrantIssuedReport/j:Warrant[@structures:id=/wir-doc:WarrantIssuedReport/j:ActivityWarrantAssociation/j:Warrant/@structures:ref]/j:CourtOrderEnforcementAgency/wir-ext:AgencyRecordIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>TCN345665</t>
+  </si>
+  <si>
+    <t>wir-doc:WarrantIssuedReport/j:Warrant[@structures:id=/wir-doc:WarrantIssuedReport/j:ActivityWarrantAssociation/j:Warrant/@structures:ref]/wir-ext:WarrantAugmentation/scr:TransactionControlNumberIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>Additional Warrant Information Text</t>
+  </si>
+  <si>
+    <t>Additional information about a warrant.</t>
+  </si>
+  <si>
+    <t>Additional Warrant Information</t>
+  </si>
+  <si>
+    <t>Warrant Entry Category Code Text</t>
+  </si>
+  <si>
+    <t>A type of warrant entry</t>
+  </si>
+  <si>
+    <t>Entry</t>
+  </si>
+  <si>
+    <t>wir-doc:WarrantIssuedReport/j:Warrant[@structures:id=/wir-doc:WarrantIssuedReport/j:ActivityWarrantAssociation/j:Warrant/@structures:ref]/wir-ext:WarrantAugmentation/wir-ext:WarrantAdditionalInformationText</t>
+  </si>
+  <si>
+    <t>wir-doc:WarrantIssuedReport/j:Warrant[@structures:id=/wir-doc:WarrantIssuedReport/j:ActivityWarrantAssociation/j:Warrant/@structures:ref]/wir-doc:WarrantIssuedReport/j:Warrant[@structures:id=/wir-doc:WarrantIssuedReport/j:ActivityWarrantAssociation/j:Warrant/@structures:ref]/wir-ext:WarrantAugmentation/wir-ext:WarrantAdditionalInformationText</t>
   </si>
 </sst>
 </file>
@@ -865,7 +823,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -889,12 +847,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -905,7 +857,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="880">
+  <cellStyleXfs count="898">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1786,8 +1738,26 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1843,13 +1813,7 @@
     <xf numFmtId="14" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1858,20 +1822,14 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="880">
+  <cellStyles count="898">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -2311,6 +2269,15 @@
     <cellStyle name="Followed Hyperlink" xfId="875" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="877" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="879" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="881" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="883" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="885" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="887" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="889" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="891" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="893" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="895" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="897" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -2750,6 +2717,15 @@
     <cellStyle name="Hyperlink" xfId="874" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="876" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="878" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="880" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="882" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="884" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="886" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="888" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="890" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="892" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="894" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="896" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -3085,11 +3061,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F300"/>
+  <dimension ref="A1:F294"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B25" sqref="B25"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C70" sqref="C70:F70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3105,17 +3081,17 @@
   <sheetData>
     <row r="1" spans="1:6" ht="23" customHeight="1">
       <c r="A1" s="10"/>
-      <c r="B1" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="C1" s="21"/>
+      <c r="B1" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="23"/>
       <c r="D1" s="10"/>
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="3" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>0</v>
@@ -3133,92 +3109,92 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="20" customFormat="1">
+    <row r="3" spans="1:6" s="19" customFormat="1">
       <c r="B3" s="14" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="C3" s="15"/>
       <c r="D3" s="15"/>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
     </row>
-    <row r="4" spans="1:6" s="20" customFormat="1">
+    <row r="4" spans="1:6" s="19" customFormat="1">
       <c r="C4" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="19" customFormat="1">
+      <c r="C5" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E4" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" s="20" customFormat="1">
-      <c r="C5" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="D5" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="E5" s="20" t="s">
-        <v>94</v>
-      </c>
-      <c r="F5" s="20" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" s="20" customFormat="1">
-      <c r="A6" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="C6" s="20" t="s">
+      <c r="D5" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="F5" s="19" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="19" customFormat="1">
+      <c r="A6" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="19" customFormat="1">
+      <c r="A7" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="D7" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="E7" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="E6" s="20" t="s">
-        <v>95</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" s="20" customFormat="1">
-      <c r="A7" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="C7" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="D7" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="E7" s="20" t="s">
-        <v>96</v>
-      </c>
-      <c r="F7" s="20" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" s="20" customFormat="1">
-      <c r="A8" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="C8" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="D8" s="20" t="s">
+      <c r="F7" s="19" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="19" customFormat="1">
+      <c r="A8" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="E8" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="E8" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="F8" s="20" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" s="20" customFormat="1">
+      <c r="F8" s="19" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="19" customFormat="1">
       <c r="B9" s="14" t="s">
         <v>15</v>
       </c>
@@ -3227,158 +3203,158 @@
       <c r="E9" s="15"/>
       <c r="F9" s="15"/>
     </row>
-    <row r="10" spans="1:6" s="20" customFormat="1">
+    <row r="10" spans="1:6" s="19" customFormat="1">
       <c r="B10" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="20" t="s">
+      <c r="C10" s="19" t="s">
         <v>9</v>
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="6" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" s="20" customFormat="1">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" s="19" customFormat="1">
       <c r="B11" s="6"/>
-      <c r="C11" s="20" t="s">
+      <c r="C11" s="19" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="6" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" s="20" customFormat="1">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" s="19" customFormat="1">
       <c r="B12" s="6"/>
-      <c r="C12" s="20" t="s">
+      <c r="C12" s="19" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" s="20" customFormat="1">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" s="19" customFormat="1">
       <c r="B13" s="6"/>
-      <c r="C13" s="20" t="s">
+      <c r="C13" s="19" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="6" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" s="20" customFormat="1">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" s="19" customFormat="1">
       <c r="B14" s="6"/>
-      <c r="C14" s="20" t="s">
+      <c r="C14" s="19" t="s">
         <v>25</v>
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="6" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" s="20" customFormat="1" ht="45">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="B15" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="20" t="s">
+      <c r="C15" s="19" t="s">
         <v>9</v>
       </c>
       <c r="D15" s="6"/>
       <c r="E15" s="6" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" s="20" customFormat="1" ht="45">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="B16" s="6"/>
-      <c r="C16" s="20" t="s">
+      <c r="C16" s="19" t="s">
         <v>10</v>
       </c>
       <c r="D16" s="6"/>
       <c r="E16" s="6" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" s="20" customFormat="1" ht="45">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" s="19" customFormat="1" ht="45">
       <c r="B17" s="6"/>
-      <c r="C17" s="20" t="s">
+      <c r="C17" s="19" t="s">
         <v>11</v>
       </c>
       <c r="D17" s="6"/>
       <c r="E17" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="F17" s="20" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" s="20" customFormat="1" ht="45">
+        <v>94</v>
+      </c>
+      <c r="F17" s="19" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" s="19" customFormat="1" ht="45">
       <c r="B18" s="6"/>
-      <c r="C18" s="20" t="s">
+      <c r="C18" s="19" t="s">
         <v>12</v>
       </c>
       <c r="D18" s="6"/>
       <c r="E18" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="F18" s="20" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" s="20" customFormat="1" ht="45">
+        <v>90</v>
+      </c>
+      <c r="F18" s="19" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" s="19" customFormat="1" ht="45">
       <c r="B19" s="6"/>
-      <c r="C19" s="20" t="s">
+      <c r="C19" s="19" t="s">
         <v>25</v>
       </c>
       <c r="D19" s="6"/>
       <c r="E19" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="F19" s="20" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" s="20" customFormat="1">
+        <v>95</v>
+      </c>
+      <c r="F19" s="19" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" s="19" customFormat="1">
       <c r="B20" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C20" s="24" t="s">
-        <v>146</v>
-      </c>
-      <c r="D20" s="20" t="s">
-        <v>241</v>
+      <c r="C20" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="D20" s="19" t="s">
+        <v>200</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" s="20" customFormat="1">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" s="19" customFormat="1">
       <c r="B21" s="7"/>
       <c r="C21" s="7" t="s">
         <v>4</v>
@@ -3388,61 +3364,58 @@
         <v>23235</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" s="20" customFormat="1">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" s="19" customFormat="1">
       <c r="B22" s="7"/>
-      <c r="C22" s="25" t="s">
-        <v>153</v>
-      </c>
-      <c r="D22" s="20" t="s">
-        <v>242</v>
+      <c r="C22" s="7" t="s">
+        <v>209</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6" s="20" customFormat="1">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" s="19" customFormat="1">
       <c r="B23" s="7"/>
-      <c r="C23" s="25" t="s">
-        <v>152</v>
+      <c r="C23" s="7" t="s">
+        <v>210</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6" s="20" customFormat="1">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" s="19" customFormat="1">
       <c r="B24" s="7"/>
       <c r="C24" s="7" t="s">
-        <v>154</v>
+        <v>138</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6" s="20" customFormat="1">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" s="19" customFormat="1">
       <c r="B25" s="7"/>
-      <c r="C25" s="25" t="s">
-        <v>155</v>
+      <c r="C25" s="7" t="s">
+        <v>212</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6" s="20" customFormat="1">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" s="19" customFormat="1">
       <c r="B26" s="7"/>
       <c r="C26" s="7" t="s">
         <v>16</v>
@@ -3452,43 +3425,47 @@
         <v>354786908</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="27" spans="2:6" s="20" customFormat="1">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" s="19" customFormat="1">
       <c r="B27" s="7"/>
-      <c r="C27" s="25" t="s">
-        <v>243</v>
+      <c r="C27" s="7" t="s">
+        <v>201</v>
       </c>
       <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-    </row>
-    <row r="28" spans="2:6" s="20" customFormat="1">
+      <c r="E27" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" s="19" customFormat="1">
       <c r="B28" s="7"/>
       <c r="C28" s="7" t="s">
-        <v>156</v>
+        <v>139</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="29" spans="2:6" s="20" customFormat="1">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" s="19" customFormat="1">
       <c r="B29" s="7"/>
       <c r="C29" s="7" t="s">
-        <v>157</v>
+        <v>140</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="30" spans="2:6" s="20" customFormat="1">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" s="19" customFormat="1">
       <c r="B30" s="7"/>
       <c r="C30" s="7" t="s">
         <v>21</v>
@@ -3498,23 +3475,23 @@
         <v>71</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="31" spans="2:6" s="20" customFormat="1">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" s="19" customFormat="1">
       <c r="B31" s="7"/>
       <c r="C31" s="7" t="s">
         <v>22</v>
       </c>
       <c r="D31" s="7"/>
       <c r="E31" s="7" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="32" spans="2:6" s="20" customFormat="1">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" s="19" customFormat="1">
       <c r="B32" s="7"/>
       <c r="C32" s="7" t="s">
         <v>23</v>
@@ -3524,47 +3501,47 @@
         <v>165</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" s="20" customFormat="1">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" s="19" customFormat="1">
       <c r="B33" s="7"/>
       <c r="C33" s="7" t="s">
         <v>24</v>
       </c>
       <c r="D33" s="7"/>
       <c r="E33" s="7" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" s="20" customFormat="1">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" s="19" customFormat="1">
       <c r="B34" s="7"/>
       <c r="C34" s="7" t="s">
-        <v>158</v>
+        <v>141</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" s="20" customFormat="1">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" s="19" customFormat="1">
       <c r="B35" s="7"/>
       <c r="C35" s="7" t="s">
-        <v>159</v>
+        <v>142</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" s="20" customFormat="1">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" s="19" customFormat="1">
       <c r="B36" s="7"/>
       <c r="C36" s="7" t="s">
         <v>6</v>
@@ -3574,635 +3551,599 @@
         <v>98213455</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" s="20" customFormat="1" ht="30">
-      <c r="A37" s="20" t="s">
-        <v>39</v>
+        <v>162</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" s="19" customFormat="1" ht="30">
+      <c r="A37" s="19" t="s">
+        <v>37</v>
       </c>
       <c r="B37" s="7"/>
       <c r="C37" s="7" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" s="20" customFormat="1">
-      <c r="A38" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="B38" s="7" t="s">
-        <v>249</v>
-      </c>
-      <c r="C38" s="27" t="s">
-        <v>57</v>
+        <v>163</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" s="19" customFormat="1">
+      <c r="A38" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B38" s="7"/>
+      <c r="C38" s="7" t="s">
+        <v>63</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" s="20" customFormat="1">
-      <c r="A39" s="20" t="s">
-        <v>39</v>
+        <v>164</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" s="19" customFormat="1">
+      <c r="A39" s="19" t="s">
+        <v>37</v>
       </c>
       <c r="B39" s="7"/>
       <c r="C39" s="7" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="E39" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="F39" s="7" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="B40" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C40" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="F40" s="6" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="B41" s="6"/>
+      <c r="C41" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="F41" s="6" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" s="19" customFormat="1">
+      <c r="B42" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C42" s="15"/>
+      <c r="D42" s="15"/>
+      <c r="E42" s="15"/>
+      <c r="F42" s="15"/>
+    </row>
+    <row r="43" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="C43" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E43" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="F43" s="6" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="C44" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="E44" s="19" t="s">
         <v>120</v>
       </c>
-      <c r="F39" s="7" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" s="20" customFormat="1">
-      <c r="A40" s="20" t="s">
+      <c r="F44" s="6" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="C45" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="E45" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="F45" s="6" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="C46" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="E46" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="F46" s="6" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="C47" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E47" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="F47" s="6" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="C48" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="D48" s="19" t="s">
+        <v>204</v>
+      </c>
+      <c r="E48" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="F48" s="6" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="C49" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="D49" s="19" t="s">
+        <v>204</v>
+      </c>
+      <c r="E49" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="F49" s="6" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="C50" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="D50" s="19" t="s">
+        <v>204</v>
+      </c>
+      <c r="E50" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="F50" s="6" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="C51" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E51" s="19">
+        <v>2012</v>
+      </c>
+      <c r="F51" s="6" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="A52" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B52" s="9"/>
+      <c r="C52" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D52" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="E52" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="F52" s="6" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" s="19" customFormat="1" ht="30">
+      <c r="B53" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C53" s="15"/>
+      <c r="D53" s="15"/>
+      <c r="E53" s="15"/>
+      <c r="F53" s="15"/>
+    </row>
+    <row r="54" spans="1:6" s="9" customFormat="1" ht="45">
+      <c r="A54" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B54" s="16"/>
+      <c r="C54" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D54" s="7"/>
+      <c r="E54" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="F54" s="6" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" s="9" customFormat="1" ht="45">
+      <c r="B55" s="16"/>
+      <c r="C55" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D55" s="7"/>
+      <c r="E55" s="7">
+        <v>6407</v>
+      </c>
+      <c r="F55" s="6" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" s="9" customFormat="1">
+      <c r="B56" s="16"/>
+      <c r="C56" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D56" s="7"/>
+      <c r="E56" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="F56" s="7"/>
+    </row>
+    <row r="57" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="C57" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E57" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="F57" s="6" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="C58" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E58" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="F58" s="6" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="C59" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E59" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="F59" s="6" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="C60" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="E60" s="19">
+        <v>63412</v>
+      </c>
+      <c r="F60" s="19" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" s="19" customFormat="1">
+      <c r="B61" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C61" s="15"/>
+      <c r="D61" s="15"/>
+      <c r="E61" s="15"/>
+      <c r="F61" s="15"/>
+    </row>
+    <row r="62" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="C62" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B40" s="7"/>
-      <c r="C40" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="D40" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="E40" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="F40" s="7" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" s="20" customFormat="1" ht="45">
-      <c r="B41" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C41" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="D41" s="6"/>
-      <c r="E41" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="F41" s="6" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" s="20" customFormat="1" ht="45">
-      <c r="B42" s="6"/>
-      <c r="C42" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D42" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E42" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="F42" s="6" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" s="20" customFormat="1">
-      <c r="B43" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="C43" s="15"/>
-      <c r="D43" s="15"/>
-      <c r="E43" s="15"/>
-      <c r="F43" s="15"/>
-    </row>
-    <row r="44" spans="1:6" s="20" customFormat="1" ht="45">
-      <c r="C44" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E44" s="20" t="s">
-        <v>131</v>
-      </c>
-      <c r="F44" s="6" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" s="20" customFormat="1" ht="45">
-      <c r="C45" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="E45" s="20" t="s">
-        <v>132</v>
-      </c>
-      <c r="F45" s="6" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" s="20" customFormat="1" ht="45">
-      <c r="C46" s="25" t="s">
-        <v>147</v>
-      </c>
-      <c r="E46" s="20" t="s">
-        <v>124</v>
-      </c>
-      <c r="F46" s="6" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" s="20" customFormat="1" ht="45">
-      <c r="C47" s="25" t="s">
-        <v>148</v>
-      </c>
-      <c r="E47" s="20" t="s">
-        <v>125</v>
-      </c>
-      <c r="F47" s="6" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" s="20" customFormat="1" ht="45">
-      <c r="C48" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E48" s="20" t="s">
-        <v>127</v>
-      </c>
-      <c r="F48" s="6" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" s="20" customFormat="1" ht="45">
-      <c r="C49" s="25" t="s">
-        <v>149</v>
-      </c>
-      <c r="D49" s="20" t="s">
-        <v>246</v>
-      </c>
-      <c r="E49" s="20" t="s">
-        <v>128</v>
-      </c>
-      <c r="F49" s="6" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" s="20" customFormat="1" ht="45">
-      <c r="C50" s="25" t="s">
-        <v>150</v>
-      </c>
-      <c r="D50" s="20" t="s">
-        <v>246</v>
-      </c>
-      <c r="E50" s="20">
-        <v>2</v>
-      </c>
-      <c r="F50" s="6" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" s="20" customFormat="1" ht="30">
-      <c r="C51" s="25" t="s">
-        <v>151</v>
-      </c>
-      <c r="D51" s="20" t="s">
-        <v>246</v>
-      </c>
-      <c r="E51" s="20" t="s">
+      <c r="D62" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="E62" s="13">
+        <v>41133</v>
+      </c>
+      <c r="F62" s="6" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" s="19" customFormat="1" ht="43" customHeight="1">
+      <c r="C63" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E63" s="19">
+        <v>5000</v>
+      </c>
+      <c r="F63" s="6" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="C64" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E64" s="13">
+        <v>40767</v>
+      </c>
+      <c r="F64" s="6" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="C65" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E65" s="19">
+        <v>659056746</v>
+      </c>
+      <c r="F65" s="6" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="C66" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="E66" s="19" t="s">
         <v>126</v>
       </c>
-      <c r="F51" s="6" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" s="20" customFormat="1" ht="45">
-      <c r="C52" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E52" s="20">
-        <v>2012</v>
-      </c>
-      <c r="F52" s="6" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" s="20" customFormat="1" ht="45">
-      <c r="A53" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="C53" s="7" t="s">
+      <c r="F66" s="6" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="A67" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C67" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="D53" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="E53" s="13">
-        <v>41174</v>
-      </c>
-      <c r="F53" s="6" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" s="20" customFormat="1" ht="45">
-      <c r="A54" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="C54" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="D54" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="E54" s="20" t="s">
-        <v>130</v>
-      </c>
-      <c r="F54" s="6" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" s="20" customFormat="1" ht="45">
-      <c r="A55" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="B55" s="9"/>
-      <c r="C55" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="D55" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="E55" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="F55" s="6" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" s="20" customFormat="1" ht="30">
-      <c r="B56" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="C56" s="15"/>
-      <c r="D56" s="15"/>
-      <c r="E56" s="15"/>
-      <c r="F56" s="15"/>
-    </row>
-    <row r="57" spans="1:6" s="9" customFormat="1" ht="45">
-      <c r="A57" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="B57" s="16"/>
-      <c r="C57" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D57" s="7"/>
-      <c r="E57" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="F57" s="6" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" s="9" customFormat="1" ht="45">
-      <c r="B58" s="16"/>
-      <c r="C58" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D58" s="7"/>
-      <c r="E58" s="7">
-        <v>6407</v>
-      </c>
-      <c r="F58" s="6" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" s="9" customFormat="1">
-      <c r="B59" s="16"/>
-      <c r="C59" s="7" t="s">
+      <c r="D67" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="E67" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="F67" s="6" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" s="19" customFormat="1" ht="60">
+      <c r="A68" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="D59" s="7"/>
-      <c r="E59" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="F59" s="7"/>
-    </row>
-    <row r="60" spans="1:6" s="20" customFormat="1" ht="45">
-      <c r="C60" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E60" s="20" t="s">
-        <v>133</v>
-      </c>
-      <c r="F60" s="6" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" s="20" customFormat="1" ht="45">
-      <c r="C61" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E61" s="20" t="s">
-        <v>136</v>
-      </c>
-      <c r="F61" s="6" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" s="20" customFormat="1" ht="45">
-      <c r="C62" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E62" s="20" t="s">
-        <v>137</v>
-      </c>
-      <c r="F62" s="6" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" s="20" customFormat="1" ht="45">
-      <c r="C63" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="E63" s="20" t="s">
-        <v>138</v>
-      </c>
-      <c r="F63" s="20" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" s="20" customFormat="1" ht="45">
-      <c r="C64" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E64" s="20">
-        <v>119</v>
-      </c>
-      <c r="F64" s="20" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" s="20" customFormat="1" ht="45">
-      <c r="C65" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="E65" s="20">
-        <v>63412</v>
-      </c>
-      <c r="F65" s="20" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" s="20" customFormat="1">
-      <c r="B66" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="C66" s="15"/>
-      <c r="D66" s="15"/>
-      <c r="E66" s="15"/>
-      <c r="F66" s="15"/>
-    </row>
-    <row r="67" spans="1:6" s="20" customFormat="1" ht="45">
-      <c r="C67" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="D67" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="E67" s="13">
-        <v>41133</v>
-      </c>
-      <c r="F67" s="6" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" s="20" customFormat="1" ht="43" customHeight="1">
       <c r="C68" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="E68" s="20">
-        <v>5000</v>
+      <c r="D68" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="E68" s="19" t="s">
+        <v>128</v>
       </c>
       <c r="F68" s="6" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" s="20" customFormat="1" ht="45">
-      <c r="C69" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E69" s="13">
-        <v>40767</v>
+        <v>192</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="C69" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D69" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="E69" s="19">
+        <v>758075800</v>
       </c>
       <c r="F69" s="6" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" s="20" customFormat="1" ht="45">
-      <c r="C70" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="E70" s="20">
-        <v>659056746</v>
+        <v>193</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="A70" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B70" s="20"/>
+      <c r="C70" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="D70" s="20" t="s">
+        <v>223</v>
+      </c>
+      <c r="E70" s="19" t="s">
+        <v>224</v>
       </c>
       <c r="F70" s="6" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" s="20" customFormat="1" ht="45">
-      <c r="C71" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="E71" s="20" t="s">
-        <v>139</v>
-      </c>
-      <c r="F71" s="6" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" s="20" customFormat="1" ht="45">
-      <c r="A72" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="C72" s="7" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="C71" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="D71" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="E71" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="F71" s="19" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="A72" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B72" s="21"/>
+      <c r="C72" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="D72" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E72" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F72" s="19" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="A73" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B73" s="9"/>
+      <c r="C73" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="D73" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="E73" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="F73" s="19" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="A74" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B74" s="9"/>
+      <c r="C74" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="D74" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="D72" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="E72" s="20" t="b">
-        <v>1</v>
-      </c>
-      <c r="F72" s="6" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" s="20" customFormat="1" ht="60">
-      <c r="A73" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="C73" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="D73" s="20" t="s">
-        <v>82</v>
-      </c>
-      <c r="E73" s="20" t="s">
-        <v>141</v>
-      </c>
-      <c r="F73" s="6" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" s="20" customFormat="1" ht="45">
-      <c r="C74" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="D74" s="20" t="s">
-        <v>87</v>
-      </c>
-      <c r="E74" s="20">
-        <v>758075800</v>
-      </c>
-      <c r="F74" s="6" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" s="20" customFormat="1">
-      <c r="A75" s="26" t="s">
-        <v>39</v>
+      <c r="E74" s="9">
+        <v>500</v>
+      </c>
+      <c r="F74" s="19" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" s="19" customFormat="1" ht="45">
+      <c r="A75" s="19" t="s">
+        <v>37</v>
       </c>
       <c r="C75" s="19" t="s">
-        <v>247</v>
-      </c>
-      <c r="D75" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="F75" s="6"/>
-    </row>
-    <row r="76" spans="1:6" s="20" customFormat="1" ht="45">
+        <v>73</v>
+      </c>
+      <c r="D75" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="E75" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="F75" s="19" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" s="19" customFormat="1" ht="45">
       <c r="C76" s="20" t="s">
-        <v>92</v>
+        <v>202</v>
       </c>
       <c r="D76" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="E76" s="20" t="s">
-        <v>140</v>
+        <v>203</v>
+      </c>
+      <c r="E76" s="19" t="s">
+        <v>226</v>
       </c>
       <c r="F76" s="20" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" s="20" customFormat="1" ht="45">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" s="22" customFormat="1" ht="45">
       <c r="A77" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="B77" s="23" t="s">
-        <v>240</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="B77" s="21"/>
       <c r="C77" s="9" t="s">
-        <v>81</v>
+        <v>228</v>
       </c>
       <c r="D77" s="9" t="s">
-        <v>51</v>
+        <v>229</v>
       </c>
       <c r="E77" s="9" t="s">
-        <v>142</v>
+        <v>230</v>
       </c>
       <c r="F77" s="20" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" s="20" customFormat="1" ht="45">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" s="22" customFormat="1" ht="75">
       <c r="A78" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="B78" s="9"/>
-      <c r="C78" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="D78" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="E78" s="9" t="s">
-        <v>122</v>
+        <v>37</v>
+      </c>
+      <c r="C78" s="20" t="s">
+        <v>231</v>
+      </c>
+      <c r="D78" s="20" t="s">
+        <v>232</v>
+      </c>
+      <c r="E78" s="20" t="s">
+        <v>233</v>
       </c>
       <c r="F78" s="20" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" s="20" customFormat="1" ht="45">
-      <c r="A79" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="B79" s="9"/>
-      <c r="C79" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="D79" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="E79" s="9">
-        <v>500</v>
-      </c>
-      <c r="F79" s="20" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" s="20" customFormat="1" ht="45">
-      <c r="A80" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="C80" s="20" t="s">
-        <v>84</v>
-      </c>
-      <c r="D80" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="E80" s="20" t="s">
-        <v>143</v>
-      </c>
-      <c r="F80" s="20" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="81" spans="2:6" s="20" customFormat="1" ht="71" customHeight="1">
-      <c r="B81" s="22"/>
-      <c r="C81" s="22"/>
-      <c r="D81" s="22"/>
-      <c r="E81" s="22"/>
-      <c r="F81" s="22"/>
-    </row>
-    <row r="82" spans="2:6" s="20" customFormat="1">
-      <c r="C82" s="26" t="s">
-        <v>244</v>
-      </c>
-      <c r="D82" s="26" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="83" spans="2:6" s="20" customFormat="1"/>
-    <row r="84" spans="2:6" s="20" customFormat="1"/>
-    <row r="85" spans="2:6" s="20" customFormat="1">
-      <c r="B85" s="26" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="86" spans="2:6" s="20" customFormat="1"/>
-    <row r="87" spans="2:6" s="20" customFormat="1"/>
+        <v>235</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" s="19" customFormat="1">
+      <c r="B79" s="22"/>
+    </row>
+    <row r="80" spans="1:6" s="19" customFormat="1"/>
+    <row r="81" s="19" customFormat="1"/>
+    <row r="281" hidden="1"/>
+    <row r="282" hidden="1"/>
+    <row r="283" hidden="1"/>
+    <row r="284" hidden="1"/>
+    <row r="285" hidden="1"/>
+    <row r="286" hidden="1"/>
     <row r="287" hidden="1"/>
     <row r="288" hidden="1"/>
     <row r="289" hidden="1"/>
@@ -4211,16 +4152,9 @@
     <row r="292" hidden="1"/>
     <row r="293" hidden="1"/>
     <row r="294" hidden="1"/>
-    <row r="295" hidden="1"/>
-    <row r="296" hidden="1"/>
-    <row r="297" hidden="1"/>
-    <row r="298" hidden="1"/>
-    <row r="299" hidden="1"/>
-    <row r="300" hidden="1"/>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="1">
     <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B81:F81"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4235,10 +4169,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G86"/>
+  <dimension ref="A1:G85"/>
   <sheetViews>
-    <sheetView topLeftCell="C8" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4255,10 +4189,10 @@
   <sheetData>
     <row r="1" spans="1:7" ht="23" customHeight="1">
       <c r="A1" s="10"/>
-      <c r="B1" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="C1" s="21"/>
+      <c r="B1" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="23"/>
       <c r="D1" s="10"/>
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
@@ -4266,7 +4200,7 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="3" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>0</v>
@@ -4288,7 +4222,7 @@
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="20"/>
+      <c r="A3" s="19"/>
       <c r="B3" s="4" t="s">
         <v>15</v>
       </c>
@@ -4298,61 +4232,55 @@
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="1:7" s="20" customFormat="1" ht="45">
+    <row r="4" spans="1:7" s="19" customFormat="1" ht="45">
       <c r="B4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="19" t="s">
         <v>9</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" s="20" customFormat="1" ht="45">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="19" customFormat="1">
       <c r="B5" s="6"/>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="19" t="s">
         <v>10</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" s="20" customFormat="1" ht="45">
+        <v>88</v>
+      </c>
+      <c r="F5" s="6"/>
+    </row>
+    <row r="6" spans="1:7" s="19" customFormat="1">
       <c r="B6" s="6"/>
-      <c r="C6" s="20" t="s">
+      <c r="C6" s="19" t="s">
         <v>11</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" s="20" customFormat="1" ht="45">
+        <v>89</v>
+      </c>
+      <c r="F6" s="6"/>
+    </row>
+    <row r="7" spans="1:7" s="19" customFormat="1">
       <c r="B7" s="6"/>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="19" t="s">
         <v>12</v>
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" s="20" customFormat="1" ht="45">
+        <v>90</v>
+      </c>
+      <c r="F7" s="6"/>
+    </row>
+    <row r="8" spans="1:7" s="19" customFormat="1">
       <c r="B8" s="7"/>
       <c r="C8" s="7" t="s">
         <v>4</v>
@@ -4361,328 +4289,307 @@
       <c r="E8" s="18">
         <v>23235</v>
       </c>
-      <c r="F8" s="6" t="s">
-        <v>234</v>
-      </c>
+      <c r="F8" s="6"/>
       <c r="G8" s="9"/>
     </row>
-    <row r="9" spans="1:7" s="20" customFormat="1" ht="45">
+    <row r="9" spans="1:7" s="19" customFormat="1">
       <c r="B9" s="7"/>
       <c r="C9" s="7" t="s">
-        <v>152</v>
+        <v>210</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>235</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="F9" s="6"/>
       <c r="G9" s="9"/>
     </row>
-    <row r="10" spans="1:7" s="20" customFormat="1" ht="45">
+    <row r="10" spans="1:7" s="19" customFormat="1">
       <c r="B10" s="7"/>
       <c r="C10" s="7" t="s">
-        <v>155</v>
+        <v>212</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>236</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="F10" s="6"/>
       <c r="G10" s="9"/>
     </row>
-    <row r="11" spans="1:7" s="20" customFormat="1" ht="45">
-      <c r="B11" s="7"/>
-      <c r="C11" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>237</v>
-      </c>
-      <c r="G11" s="9"/>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="20"/>
-      <c r="B12" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="8"/>
-    </row>
-    <row r="13" spans="1:7" s="20" customFormat="1" ht="45">
+    <row r="11" spans="1:7">
+      <c r="A11" s="19"/>
+      <c r="B11" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="8"/>
+    </row>
+    <row r="12" spans="1:7" s="19" customFormat="1">
+      <c r="C12" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12" s="19">
+        <v>758075800</v>
+      </c>
+      <c r="F12" s="6"/>
+    </row>
+    <row r="13" spans="1:7" s="22" customFormat="1">
       <c r="C13" s="6" t="s">
-        <v>48</v>
+        <v>205</v>
       </c>
       <c r="D13" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="E13" s="20">
-        <v>758075800</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" s="20" customFormat="1">
+        <v>223</v>
+      </c>
+      <c r="E13" s="20" t="s">
+        <v>224</v>
+      </c>
+      <c r="F13" s="6"/>
+    </row>
+    <row r="14" spans="1:7" s="12" customFormat="1">
+      <c r="A14" s="19"/>
       <c r="C14" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="D14" s="12"/>
+        <v>81</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>127</v>
+      </c>
       <c r="F14" s="6"/>
     </row>
-    <row r="15" spans="1:7" s="12" customFormat="1" ht="30">
-      <c r="A15" s="20"/>
-      <c r="C15" s="20" t="s">
-        <v>92</v>
-      </c>
-      <c r="D15" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="E15" s="20" t="s">
-        <v>140</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" s="20" customFormat="1"/>
-    <row r="17" spans="1:1" s="20" customFormat="1"/>
-    <row r="18" spans="1:1" s="20" customFormat="1"/>
-    <row r="19" spans="1:1" s="20" customFormat="1"/>
-    <row r="20" spans="1:1" s="20" customFormat="1"/>
-    <row r="21" spans="1:1" s="20" customFormat="1"/>
-    <row r="22" spans="1:1" s="20" customFormat="1"/>
+    <row r="15" spans="1:7" s="19" customFormat="1"/>
+    <row r="16" spans="1:7" s="19" customFormat="1"/>
+    <row r="17" spans="1:1" s="19" customFormat="1"/>
+    <row r="18" spans="1:1" s="19" customFormat="1"/>
+    <row r="19" spans="1:1" s="19" customFormat="1"/>
+    <row r="20" spans="1:1" s="19" customFormat="1"/>
+    <row r="21" spans="1:1" s="19" customFormat="1"/>
+    <row r="22" spans="1:1">
+      <c r="A22" s="19"/>
+    </row>
     <row r="23" spans="1:1">
-      <c r="A23" s="20"/>
+      <c r="A23" s="19"/>
     </row>
     <row r="24" spans="1:1">
-      <c r="A24" s="20"/>
+      <c r="A24" s="19"/>
     </row>
     <row r="25" spans="1:1">
-      <c r="A25" s="20"/>
+      <c r="A25" s="19"/>
     </row>
     <row r="26" spans="1:1">
-      <c r="A26" s="20"/>
+      <c r="A26" s="19"/>
     </row>
     <row r="27" spans="1:1">
-      <c r="A27" s="20"/>
+      <c r="A27" s="19"/>
     </row>
     <row r="28" spans="1:1">
-      <c r="A28" s="20"/>
+      <c r="A28" s="19"/>
     </row>
     <row r="29" spans="1:1">
-      <c r="A29" s="20"/>
+      <c r="A29" s="19"/>
     </row>
     <row r="30" spans="1:1">
-      <c r="A30" s="20"/>
+      <c r="A30" s="19"/>
     </row>
     <row r="31" spans="1:1">
-      <c r="A31" s="20"/>
+      <c r="A31" s="19"/>
     </row>
     <row r="32" spans="1:1">
-      <c r="A32" s="20"/>
+      <c r="A32" s="19"/>
     </row>
     <row r="33" spans="1:1">
-      <c r="A33" s="20"/>
+      <c r="A33" s="19"/>
     </row>
     <row r="34" spans="1:1">
-      <c r="A34" s="20"/>
+      <c r="A34" s="19"/>
     </row>
     <row r="35" spans="1:1">
-      <c r="A35" s="20"/>
+      <c r="A35" s="19" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="36" spans="1:1">
-      <c r="A36" s="20" t="s">
-        <v>39</v>
+      <c r="A36" s="19" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="37" spans="1:1">
-      <c r="A37" s="20" t="s">
-        <v>39</v>
+      <c r="A37" s="19" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="38" spans="1:1">
-      <c r="A38" s="20" t="s">
-        <v>39</v>
+      <c r="A38" s="19" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="39" spans="1:1">
-      <c r="A39" s="20" t="s">
-        <v>39</v>
-      </c>
+      <c r="A39" s="19"/>
     </row>
     <row r="40" spans="1:1">
-      <c r="A40" s="20"/>
+      <c r="A40" s="19"/>
     </row>
     <row r="41" spans="1:1">
-      <c r="A41" s="20"/>
+      <c r="A41" s="19"/>
     </row>
     <row r="42" spans="1:1">
-      <c r="A42" s="20"/>
+      <c r="A42" s="19"/>
     </row>
     <row r="43" spans="1:1">
-      <c r="A43" s="20"/>
+      <c r="A43" s="19"/>
     </row>
     <row r="44" spans="1:1">
-      <c r="A44" s="20"/>
+      <c r="A44" s="19"/>
     </row>
     <row r="45" spans="1:1">
-      <c r="A45" s="20"/>
+      <c r="A45" s="19"/>
     </row>
     <row r="46" spans="1:1">
-      <c r="A46" s="20"/>
+      <c r="A46" s="19"/>
     </row>
     <row r="47" spans="1:1">
-      <c r="A47" s="20"/>
+      <c r="A47" s="19"/>
     </row>
     <row r="48" spans="1:1">
-      <c r="A48" s="20"/>
+      <c r="A48" s="19"/>
     </row>
     <row r="49" spans="1:1">
-      <c r="A49" s="20"/>
+      <c r="A49" s="19"/>
     </row>
     <row r="50" spans="1:1">
-      <c r="A50" s="20"/>
+      <c r="A50" s="19"/>
     </row>
     <row r="51" spans="1:1">
-      <c r="A51" s="20"/>
+      <c r="A51" s="19" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="52" spans="1:1">
-      <c r="A52" s="20" t="s">
-        <v>39</v>
+      <c r="A52" s="19" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="53" spans="1:1">
-      <c r="A53" s="20" t="s">
-        <v>39</v>
+      <c r="A53" s="19" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="54" spans="1:1">
-      <c r="A54" s="20" t="s">
-        <v>39</v>
-      </c>
+      <c r="A54" s="19"/>
     </row>
     <row r="55" spans="1:1">
-      <c r="A55" s="20"/>
+      <c r="A55" s="9" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="56" spans="1:1">
-      <c r="A56" s="9" t="s">
-        <v>39</v>
-      </c>
+      <c r="A56" s="9"/>
     </row>
     <row r="57" spans="1:1">
       <c r="A57" s="9"/>
     </row>
     <row r="58" spans="1:1">
-      <c r="A58" s="9"/>
+      <c r="A58" s="19"/>
     </row>
     <row r="59" spans="1:1">
-      <c r="A59" s="20"/>
+      <c r="A59" s="19"/>
     </row>
     <row r="60" spans="1:1">
-      <c r="A60" s="20"/>
+      <c r="A60" s="19"/>
     </row>
     <row r="61" spans="1:1">
-      <c r="A61" s="20"/>
+      <c r="A61" s="19"/>
     </row>
     <row r="62" spans="1:1">
-      <c r="A62" s="20"/>
+      <c r="A62" s="19"/>
     </row>
     <row r="63" spans="1:1">
-      <c r="A63" s="20"/>
+      <c r="A63" s="19"/>
     </row>
     <row r="64" spans="1:1">
-      <c r="A64" s="20"/>
+      <c r="A64" s="19"/>
     </row>
     <row r="65" spans="1:1">
-      <c r="A65" s="20"/>
+      <c r="A65" s="19"/>
     </row>
     <row r="66" spans="1:1">
-      <c r="A66" s="20"/>
+      <c r="A66" s="19"/>
     </row>
     <row r="67" spans="1:1">
-      <c r="A67" s="20"/>
+      <c r="A67" s="19"/>
     </row>
     <row r="68" spans="1:1">
-      <c r="A68" s="20"/>
+      <c r="A68" s="19"/>
     </row>
     <row r="69" spans="1:1">
-      <c r="A69" s="20"/>
+      <c r="A69" s="19"/>
     </row>
     <row r="70" spans="1:1">
-      <c r="A70" s="20"/>
+      <c r="A70" s="19" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="71" spans="1:1">
-      <c r="A71" s="20" t="s">
-        <v>39</v>
+      <c r="A71" s="19" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="72" spans="1:1">
-      <c r="A72" s="20" t="s">
-        <v>39</v>
-      </c>
+      <c r="A72" s="19"/>
     </row>
     <row r="73" spans="1:1">
-      <c r="A73" s="20"/>
+      <c r="A73" s="19"/>
     </row>
     <row r="74" spans="1:1">
-      <c r="A74" s="20"/>
+      <c r="A74" s="19"/>
     </row>
     <row r="75" spans="1:1">
-      <c r="A75" s="20"/>
+      <c r="A75" s="19" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="76" spans="1:1">
-      <c r="A76" s="20" t="s">
-        <v>39</v>
+      <c r="A76" s="19" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="77" spans="1:1">
-      <c r="A77" s="20" t="s">
-        <v>39</v>
+      <c r="A77" s="19" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="78" spans="1:1">
-      <c r="A78" s="20" t="s">
-        <v>39</v>
+      <c r="A78" s="19" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="79" spans="1:1">
-      <c r="A79" s="20" t="s">
-        <v>39</v>
-      </c>
+      <c r="A79" s="19"/>
     </row>
     <row r="80" spans="1:1">
-      <c r="A80" s="20"/>
+      <c r="A80" s="19"/>
     </row>
     <row r="81" spans="1:1">
-      <c r="A81" s="20"/>
+      <c r="A81" s="19"/>
     </row>
     <row r="82" spans="1:1">
-      <c r="A82" s="20"/>
+      <c r="A82" s="19"/>
     </row>
     <row r="83" spans="1:1">
-      <c r="A83" s="20"/>
+      <c r="A83" s="19"/>
     </row>
     <row r="84" spans="1:1">
-      <c r="A84" s="20"/>
+      <c r="A84" s="19"/>
     </row>
     <row r="85" spans="1:1">
-      <c r="A85" s="20"/>
-    </row>
-    <row r="86" spans="1:1">
-      <c r="A86" s="20"/>
+      <c r="A85" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Updated new Warrant SSPs.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Warrant_Issued_Reporting/artifacts/service_model/information_model/IEPD/documentation/Mapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Warrant_Issued_Reporting/artifacts/service_model/information_model/IEPD/documentation/Mapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-26960" yWindow="6880" windowWidth="25600" windowHeight="15040" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-26960" yWindow="6880" windowWidth="25600" windowHeight="15040" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Warrant Issued Report" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="245">
   <si>
     <t>CLASS</t>
   </si>
@@ -729,6 +729,33 @@
   </si>
   <si>
     <t>wir-doc:WarrantIssuedReport/j:Warrant[@structures:id=/wir-doc:WarrantIssuedReport/j:ActivityWarrantAssociation/j:Warrant/@structures:ref]/wir-doc:WarrantIssuedReport/j:Warrant[@structures:id=/wir-doc:WarrantIssuedReport/j:ActivityWarrantAssociation/j:Warrant/@structures:ref]/wir-ext:WarrantAugmentation/wir-ext:WarrantAdditionalInformationText</t>
+  </si>
+  <si>
+    <t>war-doc:WarrantAcceptedReport/nc:Person[@structures:id=/war-doc:WarrantAcceptedReport/j:Warrant/j:CourtOrderDesignatedSubject/nc:RoleOfPerson/@structures:ref]/nc:PersonName/nc:PersonMiddleName</t>
+  </si>
+  <si>
+    <t>war-doc:WarrantAcceptedReport/nc:Person[@structures:id=/war-doc:WarrantAcceptedReport/j:Warrant/j:CourtOrderDesignatedSubject/nc:RoleOfPerson/@structures:ref]/nc:PersonName/nc:PersonSurName</t>
+  </si>
+  <si>
+    <t>war-doc:WarrantAcceptedReport/nc:Person[@structures:id=/war-doc:WarrantAcceptedReport/j:Warrant/j:CourtOrderDesignatedSubject/nc:RoleOfPerson/@structures:ref]/nc:PersonName/nc:PersonNameSuffixText</t>
+  </si>
+  <si>
+    <t>war-doc:WarrantAcceptedReport/nc:Person[@structures:id=/war-doc:WarrantAcceptedReport/j:Warrant/j:CourtOrderDesignatedSubject/nc:RoleOfPerson/@structures:ref]/nc:PersonBirthDate/nc:Date</t>
+  </si>
+  <si>
+    <t>war-doc:WarrantAcceptedReport/nc:Person[@structures:id=/war-doc:WarrantAcceptedReport/j:Warrant/j:CourtOrderDesignatedSubject/nc:RoleOfPerson/@structures:ref]/j:PersonRaceCode</t>
+  </si>
+  <si>
+    <t>war-doc:WarrantAcceptedReport/nc:Person[@structures:id=/war-doc:WarrantAcceptedReport/j:Warrant/j:CourtOrderDesignatedSubject/nc:RoleOfPerson/@structures:ref]/j:PersonSexCode</t>
+  </si>
+  <si>
+    <t>war-doc:WarrantAcceptedReport/j:Warrant/j:CourtOrderEnforcementAgency/j:OrganizationAugmentation/j:OrganizationORIIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>war-doc:WarrantAcceptedReport/j:Warrant/j:CourtOrderEnforcementAgency/wir-ext:AgencyRecordIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>war-doc:WarrantAcceptedReport/j:Warrant/j:CourtOrderRequestEntity/nc:EntityPerson/wir-ext:PersonEmployeeIdentification/nc:IdentificationID</t>
   </si>
 </sst>
 </file>
@@ -857,9 +884,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="898">
+  <cellStyleXfs count="906">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1829,7 +1864,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="898">
+  <cellStyles count="906">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -2278,6 +2313,10 @@
     <cellStyle name="Followed Hyperlink" xfId="893" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="895" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="897" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="899" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="901" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="903" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="905" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -2726,6 +2765,10 @@
     <cellStyle name="Hyperlink" xfId="892" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="894" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="896" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="898" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="900" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="902" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="904" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -3063,8 +3106,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F294"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C70" sqref="C70:F70"/>
     </sheetView>
   </sheetViews>
@@ -4171,8 +4214,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4247,7 +4290,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="19" customFormat="1">
+    <row r="5" spans="1:7" s="19" customFormat="1" ht="45">
       <c r="B5" s="6"/>
       <c r="C5" s="19" t="s">
         <v>10</v>
@@ -4256,9 +4299,11 @@
       <c r="E5" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="F5" s="6"/>
-    </row>
-    <row r="6" spans="1:7" s="19" customFormat="1">
+      <c r="F5" s="6" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="19" customFormat="1" ht="45">
       <c r="B6" s="6"/>
       <c r="C6" s="19" t="s">
         <v>11</v>
@@ -4267,9 +4312,11 @@
       <c r="E6" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="F6" s="6"/>
-    </row>
-    <row r="7" spans="1:7" s="19" customFormat="1">
+      <c r="F6" s="20" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="19" customFormat="1" ht="45">
       <c r="B7" s="6"/>
       <c r="C7" s="19" t="s">
         <v>12</v>
@@ -4278,9 +4325,11 @@
       <c r="E7" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="F7" s="6"/>
-    </row>
-    <row r="8" spans="1:7" s="19" customFormat="1">
+      <c r="F7" s="20" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="19" customFormat="1" ht="45">
       <c r="B8" s="7"/>
       <c r="C8" s="7" t="s">
         <v>4</v>
@@ -4289,10 +4338,12 @@
       <c r="E8" s="18">
         <v>23235</v>
       </c>
-      <c r="F8" s="6"/>
+      <c r="F8" s="20" t="s">
+        <v>239</v>
+      </c>
       <c r="G8" s="9"/>
     </row>
-    <row r="9" spans="1:7" s="19" customFormat="1">
+    <row r="9" spans="1:7" s="19" customFormat="1" ht="45">
       <c r="B9" s="7"/>
       <c r="C9" s="7" t="s">
         <v>210</v>
@@ -4301,10 +4352,12 @@
       <c r="E9" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="F9" s="6"/>
+      <c r="F9" s="20" t="s">
+        <v>240</v>
+      </c>
       <c r="G9" s="9"/>
     </row>
-    <row r="10" spans="1:7" s="19" customFormat="1">
+    <row r="10" spans="1:7" s="19" customFormat="1" ht="45">
       <c r="B10" s="7"/>
       <c r="C10" s="7" t="s">
         <v>212</v>
@@ -4313,7 +4366,9 @@
       <c r="E10" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="F10" s="6"/>
+      <c r="F10" s="20" t="s">
+        <v>241</v>
+      </c>
       <c r="G10" s="9"/>
     </row>
     <row r="11" spans="1:7">
@@ -4327,7 +4382,7 @@
       <c r="F11" s="5"/>
       <c r="G11" s="8"/>
     </row>
-    <row r="12" spans="1:7" s="19" customFormat="1">
+    <row r="12" spans="1:7" s="19" customFormat="1" ht="45">
       <c r="C12" s="6" t="s">
         <v>46</v>
       </c>
@@ -4337,9 +4392,11 @@
       <c r="E12" s="19">
         <v>758075800</v>
       </c>
-      <c r="F12" s="6"/>
-    </row>
-    <row r="13" spans="1:7" s="22" customFormat="1">
+      <c r="F12" s="6" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" s="22" customFormat="1" ht="30">
       <c r="C13" s="6" t="s">
         <v>205</v>
       </c>
@@ -4349,9 +4406,11 @@
       <c r="E13" s="20" t="s">
         <v>224</v>
       </c>
-      <c r="F13" s="6"/>
-    </row>
-    <row r="14" spans="1:7" s="12" customFormat="1">
+      <c r="F13" s="6" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="12" customFormat="1" ht="30">
       <c r="A14" s="19"/>
       <c r="C14" s="19" t="s">
         <v>81</v>
@@ -4362,7 +4421,9 @@
       <c r="E14" s="19" t="s">
         <v>127</v>
       </c>
-      <c r="F14" s="6"/>
+      <c r="F14" s="6" t="s">
+        <v>244</v>
+      </c>
     </row>
     <row r="15" spans="1:7" s="19" customFormat="1"/>
     <row r="16" spans="1:7" s="19" customFormat="1"/>

</xml_diff>